<commit_message>
change a package name
</commit_message>
<xml_diff>
--- a/AndroidStudio設計図（節約の献立管理）ver2.xlsx
+++ b/AndroidStudio設計図（節約の献立管理）ver2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shutohideto/AndroidStudioProjects/MyMenuApplication/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9084D79F-23B6-CE44-9347-80A00341D2CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A32D17-6BA8-F847-96A5-185840991C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1773A3CE-552F-2A44-9AE8-5EC860C14F84}"/>
   </bookViews>
@@ -581,48 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -681,6 +639,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -5944,7 +5944,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>合計金額</a:t>
+            <a:t>日合計金額</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6627,6 +6627,237 @@
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>年月</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="109" name="図 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B097B7B-0A83-464F-B29C-40B8FAA4B200}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="23634700" y="4775200"/>
+          <a:ext cx="1917700" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="117" name="テキスト ボックス 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{219E4D3C-7C6F-8246-87D4-6B1242082F36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="22796500" y="4889500"/>
+          <a:ext cx="1397000" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>月合計金額</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="118" name="図 117">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{312E7905-E5FC-BF45-B0E0-2CC9C487BDEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25514300" y="4775200"/>
+          <a:ext cx="1917700" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="テキスト ボックス 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD544582-0639-1F4F-8299-29816C987FD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="26898600" y="4889500"/>
+          <a:ext cx="1625600" cy="279400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>表示</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6935,8 +7166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEB4636-21A1-1647-8310-7DD9BFBF6F55}">
   <dimension ref="A1:AM36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -7266,36 +7497,36 @@
   <sheetData>
     <row r="1" spans="2:14" ht="21" thickBot="1"/>
     <row r="2" spans="2:14">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="33" t="s">
+      <c r="C2" s="16"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="23"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" spans="2:14" ht="21" thickBot="1">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="24"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="46"/>
     </row>
     <row r="4" spans="2:14" ht="21" thickTop="1">
       <c r="E4" s="1"/>
@@ -7311,216 +7542,216 @@
     </row>
     <row r="5" spans="2:14" ht="21" thickBot="1"/>
     <row r="6" spans="2:14">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="26"/>
     </row>
     <row r="7" spans="2:14" ht="21" thickBot="1">
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="9" spans="2:14" ht="21" thickBot="1"/>
     <row r="10" spans="2:14">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="44"/>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="2:14" ht="21" thickBot="1">
-      <c r="B11" s="45"/>
-      <c r="C11" s="46"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
     </row>
     <row r="19" spans="5:14" ht="21" thickBot="1"/>
     <row r="20" spans="5:14" ht="15" customHeight="1">
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="25" t="s">
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="25"/>
+      <c r="N20" s="35"/>
     </row>
     <row r="21" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
     </row>
     <row r="22" spans="5:14" ht="15" customHeight="1"/>
     <row r="24" spans="5:14" ht="21" thickBot="1"/>
     <row r="25" spans="5:14" ht="15" customHeight="1">
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="27" t="s">
+      <c r="F25" s="35"/>
+      <c r="G25" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
     </row>
     <row r="26" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="48"/>
     </row>
     <row r="27" spans="5:14" ht="15" customHeight="1"/>
     <row r="28" spans="5:14" ht="21" thickBot="1"/>
     <row r="29" spans="5:14" ht="15" customHeight="1">
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="17"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="38"/>
+      <c r="N29" s="39"/>
     </row>
     <row r="30" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E30" s="18"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="20"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="41"/>
+      <c r="K30" s="41"/>
+      <c r="L30" s="41"/>
+      <c r="M30" s="41"/>
+      <c r="N30" s="42"/>
     </row>
     <row r="31" spans="5:14" ht="15" customHeight="1">
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
-      <c r="L31" s="16"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="17"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="38"/>
+      <c r="N31" s="39"/>
     </row>
     <row r="32" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E32" s="18"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="20"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
+      <c r="J32" s="41"/>
+      <c r="K32" s="41"/>
+      <c r="L32" s="41"/>
+      <c r="M32" s="41"/>
+      <c r="N32" s="42"/>
     </row>
     <row r="33" spans="5:14" ht="15" customHeight="1">
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="17"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="39"/>
     </row>
     <row r="34" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E34" s="18"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="20"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="42"/>
     </row>
     <row r="35" spans="5:14" ht="15" customHeight="1">
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="17"/>
+      <c r="F35" s="38"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="38"/>
+      <c r="K35" s="38"/>
+      <c r="L35" s="38"/>
+      <c r="M35" s="38"/>
+      <c r="N35" s="39"/>
     </row>
     <row r="36" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E36" s="18"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="20"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="41"/>
+      <c r="G36" s="41"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="41"/>
+      <c r="K36" s="41"/>
+      <c r="L36" s="41"/>
+      <c r="M36" s="41"/>
+      <c r="N36" s="42"/>
     </row>
     <row r="37" spans="5:14" ht="15" customHeight="1">
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16"/>
-      <c r="N37" s="17"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="38"/>
+      <c r="K37" s="38"/>
+      <c r="L37" s="38"/>
+      <c r="M37" s="38"/>
+      <c r="N37" s="39"/>
     </row>
     <row r="38" spans="5:14" ht="15" customHeight="1" thickBot="1">
-      <c r="E38" s="18"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="20"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="41"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
+      <c r="K38" s="41"/>
+      <c r="L38" s="41"/>
+      <c r="M38" s="41"/>
+      <c r="N38" s="42"/>
     </row>
     <row r="39" spans="5:14" ht="15" customHeight="1"/>
     <row r="40" spans="5:14" ht="15" customHeight="1"/>
@@ -7529,12 +7760,6 @@
     <row r="43" spans="5:14" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B2:C3"/>
-    <mergeCell ref="F2:M3"/>
-    <mergeCell ref="B6:C7"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="E20:L21"/>
-    <mergeCell ref="M20:N21"/>
     <mergeCell ref="E37:N38"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="N2:N3"/>
@@ -7544,6 +7769,12 @@
     <mergeCell ref="E31:N32"/>
     <mergeCell ref="E33:N34"/>
     <mergeCell ref="E35:N36"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="F2:M3"/>
+    <mergeCell ref="B6:C7"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="E20:L21"/>
+    <mergeCell ref="M20:N21"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>